<commit_message>
Get all tests running.
</commit_message>
<xml_diff>
--- a/src/Middleware/tests/Orchestration.Tests/TemplateTests/TemplateSheets.xlsx
+++ b/src/Middleware/tests/Orchestration.Tests/TemplateTests/TemplateSheets.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HeadStart\OC-Marketplace.RyanLauer\src\Middleware\tests\Orchestration.Tests\TemplateTests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10860FD1-5950-4F71-B82C-E4C8D2E3ED67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-45" yWindow="-15330" windowWidth="21600" windowHeight="12555" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Products" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="PriceSchedules" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Specs" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="SpecOptions" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Images" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Attachments" sheetId="6" r:id="rId9"/>
+    <sheet name="Products" sheetId="1" r:id="rId1"/>
+    <sheet name="PriceSchedules" sheetId="2" r:id="rId2"/>
+    <sheet name="Specs" sheetId="3" r:id="rId3"/>
+    <sheet name="SpecOptions" sheetId="4" r:id="rId4"/>
+    <sheet name="Images" sheetId="5" r:id="rId5"/>
+    <sheet name="Attachments" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -180,9 +189,6 @@
     <t>example_spec_option_blue</t>
   </si>
   <si>
-    <t>examle_attachment</t>
-  </si>
-  <si>
     <t>Shirt</t>
   </si>
   <si>
@@ -201,36 +207,39 @@
     <t>AmountPerQuantity</t>
   </si>
   <si>
-    <t>http://pdf.url.com</t>
-  </si>
-  <si>
     <t>http://image.url.com</t>
   </si>
   <si>
-    <t>Attachment</t>
-  </si>
-  <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>example_attachment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -238,7 +247,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -248,64 +257,43 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -495,31 +483,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.57"/>
-    <col customWidth="1" min="2" max="2" width="8.43"/>
-    <col customWidth="1" min="3" max="3" width="22.71"/>
-    <col customWidth="1" min="4" max="4" width="15.43"/>
-    <col customWidth="1" min="5" max="5" width="10.57"/>
-    <col customWidth="1" min="6" max="6" width="10.29"/>
-    <col customWidth="1" min="7" max="7" width="9.57"/>
-    <col customWidth="1" min="8" max="8" width="10.57"/>
-    <col customWidth="1" min="9" max="9" width="6.14"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +557,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -577,25 +568,25 @@
         <v>36</v>
       </c>
       <c r="D2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>37</v>
@@ -604,7 +595,7 @@
         <v>38</v>
       </c>
       <c r="M2" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>39</v>
@@ -614,33 +605,34 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.43"/>
-    <col customWidth="1" min="2" max="2" width="9.43"/>
-    <col customWidth="1" min="3" max="3" width="6.14"/>
-    <col customWidth="1" min="4" max="4" width="8.71"/>
-    <col customWidth="1" min="5" max="5" width="13.0"/>
-    <col customWidth="1" min="6" max="6" width="11.0"/>
-    <col customWidth="1" min="7" max="7" width="11.57"/>
-    <col customWidth="1" min="8" max="8" width="20.71"/>
-    <col customWidth="1" min="9" max="9" width="16.43"/>
-    <col customWidth="1" min="10" max="16" width="10.29"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="16" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -707,10 +699,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="H2" s="1" t="b">
         <v>1</v>
@@ -720,32 +712,33 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.71"/>
-    <col customWidth="1" min="2" max="2" width="10.57"/>
-    <col customWidth="1" min="3" max="3" width="32.29"/>
-    <col customWidth="1" min="4" max="4" width="8.71"/>
-    <col customWidth="1" min="5" max="5" width="19.43"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="13.57"/>
-    <col customWidth="1" min="8" max="8" width="14.29"/>
-    <col customWidth="1" min="9" max="9" width="13.14"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -785,7 +778,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>1</v>
@@ -797,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -808,7 +801,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>34</v>
@@ -824,30 +817,31 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.71"/>
-    <col customWidth="1" min="2" max="2" width="20.71"/>
-    <col customWidth="1" min="3" max="3" width="5.71"/>
-    <col customWidth="1" min="4" max="4" width="8.71"/>
-    <col customWidth="1" min="5" max="5" width="10.57"/>
-    <col customWidth="1" min="6" max="6" width="15.57"/>
-    <col customWidth="1" min="7" max="7" width="11.57"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -881,57 +875,60 @@
         <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="G3" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +954,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -965,37 +962,40 @@
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,30 +1021,30 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7B8BD00E-80B9-4488-A584-B390DDF9AC29}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>